<commit_message>
feat: implement PDF export and dynamic titles for voceros, fix menu visibility
</commit_message>
<xml_diff>
--- a/database/voceros.xlsx
+++ b/database/voceros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\YanguasEjercicios\senapre\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AA3328-1BDA-42F2-97B3-0E0ADE566340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86226493-F304-47DE-B7E3-0B202D12BFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VOCEROS JORNADA DIURNA " sheetId="2" r:id="rId1"/>
@@ -2076,6 +2076,9 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2114,9 +2117,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3894,8 +3894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC979"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
@@ -4041,7 +4041,7 @@
       <c r="B4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="39">
         <v>17658004</v>
       </c>
       <c r="D4" s="38" t="s">
@@ -13401,22 +13401,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:98" s="16" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="133" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
@@ -14778,12 +14778,12 @@
       <c r="J12" s="88">
         <v>45937</v>
       </c>
-      <c r="K12" s="129" t="s">
+      <c r="K12" s="130" t="s">
         <v>171</v>
       </c>
-      <c r="L12" s="130"/>
-      <c r="M12" s="130"/>
-      <c r="N12" s="131"/>
+      <c r="L12" s="131"/>
+      <c r="M12" s="131"/>
+      <c r="N12" s="132"/>
       <c r="O12" s="40"/>
       <c r="P12" s="40"/>
       <c r="Q12" s="40"/>
@@ -32562,7 +32562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BY984"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -32585,21 +32585,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:77" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="134" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
     </row>
     <row r="2" spans="1:77" s="16" customFormat="1" ht="34.5" customHeight="1">
       <c r="A2" s="66" t="s">
@@ -32733,12 +32733,12 @@
       <c r="I3" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="J3" s="135" t="s">
+      <c r="J3" s="136" t="s">
         <v>255</v>
       </c>
-      <c r="K3" s="136"/>
-      <c r="L3" s="136"/>
-      <c r="M3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="137"/>
+      <c r="M3" s="138"/>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
@@ -32933,12 +32933,12 @@
       <c r="I5" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="J5" s="135" t="s">
+      <c r="J5" s="136" t="s">
         <v>255</v>
       </c>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="137"/>
+      <c r="K5" s="137"/>
+      <c r="L5" s="137"/>
+      <c r="M5" s="138"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
@@ -33176,12 +33176,12 @@
       <c r="I8" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="J8" s="135" t="s">
+      <c r="J8" s="136" t="s">
         <v>286</v>
       </c>
-      <c r="K8" s="136"/>
-      <c r="L8" s="136"/>
-      <c r="M8" s="137"/>
+      <c r="K8" s="137"/>
+      <c r="L8" s="137"/>
+      <c r="M8" s="138"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
@@ -33607,7 +33607,7 @@
       <c r="B16" s="20">
         <v>1117504709</v>
       </c>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="129" t="s">
         <v>415</v>
       </c>
       <c r="D16" s="20">
@@ -34892,20 +34892,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>364</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="140"/>
+      <c r="K1" s="140"/>
+      <c r="L1" s="140"/>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
       <c r="A2" s="22" t="s">
@@ -36191,17 +36191,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="141" t="s">
         <v>384</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1">
       <c r="A2" s="8" t="s">

</xml_diff>